<commit_message>
fix lop hoc+ dot thi + import điểm thi dang dở :(
</commit_message>
<xml_diff>
--- a/TemplateDiem.xlsx
+++ b/TemplateDiem.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieu1\Desktop\CaoThangAngular\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>hoten</t>
   </si>
@@ -50,15 +50,6 @@
     <t>xeploai</t>
   </si>
   <si>
-    <t>ngaythi</t>
-  </si>
-  <si>
-    <t>giothi</t>
-  </si>
-  <si>
-    <t>phongthi</t>
-  </si>
-  <si>
     <t>msword</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
     <t>Giỏi</t>
   </si>
   <si>
-    <t>18h</t>
-  </si>
-  <si>
     <t>Nguyễn Văn B</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
   </si>
   <si>
     <t>Kém</t>
-  </si>
-  <si>
-    <t>12h</t>
   </si>
   <si>
     <t>laptrinhc</t>
@@ -423,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +427,7 @@
     <col min="15" max="15" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,30 +453,21 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2">
         <v>123456789</v>
@@ -500,45 +476,36 @@
         <v>36483</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1">
-        <v>44167</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
       </c>
       <c r="K2">
-        <v>16.5</v>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>10</v>
       </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>123456789</v>
@@ -547,39 +514,30 @@
         <v>117215</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1206370</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
         <v>0</v>
       </c>
     </row>

</xml_diff>